<commit_message>
Column header in Excel files
</commit_message>
<xml_diff>
--- a/testfiles/excel-writer-style-template.xlsx
+++ b/testfiles/excel-writer-style-template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amin/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amin/projects/pentaho/pentaho-kettle/testfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,9 +26,32 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>col1</t>
+  </si>
+  <si>
+    <t>col2</t>
+  </si>
+  <si>
+    <t>col3</t>
+  </si>
+  <si>
+    <t>col4</t>
+  </si>
+  <si>
+    <t>col5</t>
+  </si>
+  <si>
+    <t>col6</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -43,6 +66,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -127,12 +158,14 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,27 +446,39 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="7"/>
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="4"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="6"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
+      <c r="A2" s="3"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>

</xml_diff>